<commit_message>
DelCo: Update test notes and times
</commit_message>
<xml_diff>
--- a/Projects/DelCo_2014_04/Test_Notes/FIRE_FA2S1C1NCX1_2_Notes_DM.xlsx
+++ b/Projects/DelCo_2014_04/Test_Notes/FIRE_FA2S1C1NCX1_2_Notes_DM.xlsx
@@ -148,8 +148,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -161,9 +165,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,7 +474,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -580,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <f>B8*60+C8+$D$5</f>
+        <f t="shared" ref="D8:D14" si="0">B8*60+C8+$D$5</f>
         <v>960</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -598,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <f>B9*60+C9+$D$5</f>
+        <f t="shared" si="0"/>
         <v>1020</v>
       </c>
       <c r="E9" t="s">
@@ -616,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <f>B10*60+C10+$D$5</f>
+        <f t="shared" si="0"/>
         <v>1140</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -634,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <f>B11*60+C11+$D$5</f>
+        <f t="shared" si="0"/>
         <v>1200</v>
       </c>
       <c r="E11" t="s">
@@ -652,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="3">
-        <f>B12*60+C12+$D$5</f>
+        <f t="shared" si="0"/>
         <v>1350</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -670,7 +678,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="3">
-        <f>B13*60+C13+$D$5</f>
+        <f t="shared" si="0"/>
         <v>1429</v>
       </c>
       <c r="E13" t="s">
@@ -678,10 +686,19 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="1">
+        <v>0.6645833333333333</v>
+      </c>
+      <c r="B14" s="3">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>57</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>1437</v>
+      </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>

</xml_diff>